<commit_message>
Added .xls for algorithm parameter tests
</commit_message>
<xml_diff>
--- a/praca/badania/badanie1.xlsx
+++ b/praca/badania/badanie1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abani\Desktop\Praca magisterska\praca\badania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399382DB-55B1-4F31-9BB4-5EA0CC79ECA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43867F7E-26C7-442B-9CEC-092B17F4EF55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-49815" yWindow="8310" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="29040" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,12 +135,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -465,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -489,51 +498,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -553,6 +517,54 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21:O21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,31 +892,31 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="21"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="29"/>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
@@ -912,37 +924,37 @@
       <c r="AC4" s="7"/>
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C5" s="22"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="14" t="s">
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="14" t="s">
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="14" t="s">
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="11" t="s">
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="12"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="25"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="7" t="s">
         <v>7</v>
@@ -953,7 +965,7 @@
       <c r="AC5" s="7"/>
     </row>
     <row r="6" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C6" s="22"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1011,7 +1023,7 @@
       <c r="V6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="W6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="X6" s="1"/>
@@ -1024,7 +1036,7 @@
       <c r="AC6" s="7"/>
     </row>
     <row r="7" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C7" s="25">
+      <c r="C7" s="10">
         <v>1</v>
       </c>
       <c r="D7" s="5">
@@ -1084,7 +1096,7 @@
       <c r="V7" s="8">
         <v>3</v>
       </c>
-      <c r="W7" s="26">
+      <c r="W7" s="11">
         <v>7</v>
       </c>
       <c r="X7" s="1"/>
@@ -1097,7 +1109,7 @@
       <c r="AC7" s="7"/>
     </row>
     <row r="8" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C8" s="25">
+      <c r="C8" s="10">
         <v>2</v>
       </c>
       <c r="D8" s="5">
@@ -1157,7 +1169,7 @@
       <c r="V8" s="8">
         <v>4</v>
       </c>
-      <c r="W8" s="26">
+      <c r="W8" s="11">
         <v>6</v>
       </c>
       <c r="X8" s="1"/>
@@ -1170,7 +1182,7 @@
       <c r="AC8" s="7"/>
     </row>
     <row r="9" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C9" s="25">
+      <c r="C9" s="10">
         <v>3</v>
       </c>
       <c r="D9" s="5">
@@ -1230,7 +1242,7 @@
       <c r="V9" s="8">
         <v>4</v>
       </c>
-      <c r="W9" s="26">
+      <c r="W9" s="11">
         <v>6</v>
       </c>
       <c r="X9" s="1"/>
@@ -1243,7 +1255,7 @@
       <c r="AC9" s="7"/>
     </row>
     <row r="10" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C10" s="25">
+      <c r="C10" s="10">
         <v>4</v>
       </c>
       <c r="D10" s="5">
@@ -1303,7 +1315,7 @@
       <c r="V10" s="8">
         <v>4</v>
       </c>
-      <c r="W10" s="26">
+      <c r="W10" s="11">
         <v>6</v>
       </c>
       <c r="X10" s="1"/>
@@ -1316,7 +1328,7 @@
       <c r="AC10" s="7"/>
     </row>
     <row r="11" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C11" s="25">
+      <c r="C11" s="10">
         <v>5</v>
       </c>
       <c r="D11" s="5">
@@ -1376,7 +1388,7 @@
       <c r="V11" s="8">
         <v>6</v>
       </c>
-      <c r="W11" s="26">
+      <c r="W11" s="11">
         <v>4</v>
       </c>
       <c r="X11" s="1"/>
@@ -1389,7 +1401,7 @@
       <c r="AC11" s="7"/>
     </row>
     <row r="12" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C12" s="25">
+      <c r="C12" s="10">
         <v>6</v>
       </c>
       <c r="D12" s="5">
@@ -1449,7 +1461,7 @@
       <c r="V12" s="8">
         <v>5</v>
       </c>
-      <c r="W12" s="26">
+      <c r="W12" s="11">
         <v>5</v>
       </c>
       <c r="X12" s="1"/>
@@ -1460,7 +1472,7 @@
       <c r="AC12" s="7"/>
     </row>
     <row r="13" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C13" s="25">
+      <c r="C13" s="10">
         <v>7</v>
       </c>
       <c r="D13" s="5">
@@ -1520,7 +1532,7 @@
       <c r="V13" s="8">
         <v>6</v>
       </c>
-      <c r="W13" s="26">
+      <c r="W13" s="11">
         <v>4</v>
       </c>
       <c r="X13" s="1"/>
@@ -1531,7 +1543,7 @@
       <c r="AC13" s="7"/>
     </row>
     <row r="14" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C14" s="25">
+      <c r="C14" s="10">
         <v>8</v>
       </c>
       <c r="D14" s="5">
@@ -1591,7 +1603,7 @@
       <c r="V14" s="8">
         <v>4</v>
       </c>
-      <c r="W14" s="26">
+      <c r="W14" s="11">
         <v>6</v>
       </c>
       <c r="X14" s="1"/>
@@ -1604,7 +1616,7 @@
       <c r="AC14" s="7"/>
     </row>
     <row r="15" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C15" s="25">
+      <c r="C15" s="10">
         <v>9</v>
       </c>
       <c r="D15" s="5">
@@ -1664,7 +1676,7 @@
       <c r="V15" s="8">
         <v>5</v>
       </c>
-      <c r="W15" s="26">
+      <c r="W15" s="11">
         <v>5</v>
       </c>
       <c r="X15" s="1"/>
@@ -1677,67 +1689,67 @@
       <c r="AC15" s="7"/>
     </row>
     <row r="16" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C16" s="27">
-        <v>10</v>
-      </c>
-      <c r="D16" s="28">
-        <v>9</v>
-      </c>
-      <c r="E16" s="29">
+      <c r="C16" s="12">
+        <v>10</v>
+      </c>
+      <c r="D16" s="13">
+        <v>9</v>
+      </c>
+      <c r="E16" s="14">
         <v>1</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="15">
         <v>5</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="15">
         <v>5</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="13">
         <v>1</v>
       </c>
-      <c r="I16" s="29">
-        <v>9</v>
-      </c>
-      <c r="J16" s="30">
-        <v>10</v>
-      </c>
-      <c r="K16" s="30">
-        <v>0</v>
-      </c>
-      <c r="L16" s="28">
+      <c r="I16" s="14">
+        <v>9</v>
+      </c>
+      <c r="J16" s="15">
+        <v>10</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0</v>
+      </c>
+      <c r="L16" s="13">
         <v>3</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="14">
         <v>7</v>
       </c>
-      <c r="N16" s="30">
-        <v>10</v>
-      </c>
-      <c r="O16" s="30">
-        <v>0</v>
-      </c>
-      <c r="P16" s="28">
+      <c r="N16" s="15">
+        <v>10</v>
+      </c>
+      <c r="O16" s="15">
+        <v>0</v>
+      </c>
+      <c r="P16" s="13">
         <v>3</v>
       </c>
-      <c r="Q16" s="29">
+      <c r="Q16" s="14">
         <v>7</v>
       </c>
-      <c r="R16" s="30">
-        <v>10</v>
-      </c>
-      <c r="S16" s="30">
-        <v>0</v>
-      </c>
-      <c r="T16" s="28">
-        <v>10</v>
-      </c>
-      <c r="U16" s="29">
-        <v>0</v>
-      </c>
-      <c r="V16" s="30">
+      <c r="R16" s="15">
+        <v>10</v>
+      </c>
+      <c r="S16" s="15">
+        <v>0</v>
+      </c>
+      <c r="T16" s="13">
+        <v>10</v>
+      </c>
+      <c r="U16" s="14">
+        <v>0</v>
+      </c>
+      <c r="V16" s="15">
         <v>5</v>
       </c>
-      <c r="W16" s="31">
+      <c r="W16" s="16">
         <v>5</v>
       </c>
       <c r="X16" s="1"/>
@@ -1750,132 +1762,132 @@
       <c r="AC16" s="7"/>
     </row>
     <row r="21" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10" t="s">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10" t="s">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10" t="s">
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="4:19" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16" t="s">
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
     </row>
     <row r="23" spans="4:19" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16" t="s">
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16" t="s">
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
     </row>
     <row r="24" spans="4:19" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16" t="s">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16" t="s">
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
     </row>
     <row r="25" spans="4:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
     </row>
     <row r="26" spans="4:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
     </row>
     <row r="27" spans="4:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
     </row>
     <row r="28" spans="4:19" ht="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="4:19" ht="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1884,14 +1896,12 @@
     <row r="32" spans="4:19" ht="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P24:S24"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="P21:S21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H27:K27"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="D22:G22"/>
@@ -1905,14 +1915,16 @@
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="P22:S22"/>
     <mergeCell ref="P23:S23"/>
+    <mergeCell ref="P24:S24"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="P21:S21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H24:K24"/>
     <mergeCell ref="L24:O24"/>
     <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H27:K27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>